<commit_message>
Chewy looks good, just needs some QTY <= 10 changes
</commit_message>
<xml_diff>
--- a/Finished/Chewy/Chewy 856 ASN PO RS41334490 11.08.2024.xlsx
+++ b/Finished/Chewy/Chewy 856 ASN PO RS41334490 11.08.2024.xlsx
@@ -1256,11 +1256,7 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D21" s="31" t="inlineStr">
-        <is>
-          <t>499.04</t>
-        </is>
-      </c>
+      <c r="D21" s="31" t="n"/>
       <c r="E21" s="31" t="inlineStr">
         <is>
           <t>850016364883</t>
@@ -1304,11 +1300,7 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D22" s="33" t="inlineStr">
-        <is>
-          <t>499.04</t>
-        </is>
-      </c>
+      <c r="D22" s="33" t="n"/>
       <c r="E22" s="31" t="inlineStr">
         <is>
           <t>850016364883</t>
@@ -1352,11 +1344,7 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D23" s="33" t="inlineStr">
-        <is>
-          <t>499.04</t>
-        </is>
-      </c>
+      <c r="D23" s="33" t="n"/>
       <c r="E23" s="31" t="inlineStr">
         <is>
           <t>850016364883</t>
@@ -1400,11 +1388,6 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>499.04</t>
-        </is>
-      </c>
       <c r="E24" t="inlineStr">
         <is>
           <t>850016364883</t>
@@ -1445,11 +1428,6 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>499.04</t>
-        </is>
-      </c>
       <c r="E25" t="inlineStr">
         <is>
           <t>850016364883</t>
@@ -1490,11 +1468,6 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>389.84</t>
-        </is>
-      </c>
       <c r="E26" t="inlineStr">
         <is>
           <t>850016364876</t>
@@ -1535,11 +1508,6 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>389.84</t>
-        </is>
-      </c>
       <c r="E27" t="inlineStr">
         <is>
           <t>850016364838</t>
@@ -1580,11 +1548,6 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>259.74</t>
-        </is>
-      </c>
       <c r="E28" t="inlineStr">
         <is>
           <t>850016364944</t>
@@ -1625,11 +1588,6 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>877.31</t>
-        </is>
-      </c>
       <c r="E29" t="inlineStr">
         <is>
           <t>860008203465</t>
@@ -1670,11 +1628,6 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>877.31</t>
-        </is>
-      </c>
       <c r="E30" t="inlineStr">
         <is>
           <t>860008203441</t>
@@ -1715,11 +1668,6 @@
           <t>45377</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>1559.81</t>
-        </is>
-      </c>
       <c r="E31" t="inlineStr">
         <is>
           <t>860008203472</t>
@@ -1758,11 +1706,6 @@
       <c r="C32" t="inlineStr">
         <is>
           <t>45377</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>584.81</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">

</xml_diff>

<commit_message>
oops mini change to QTY
</commit_message>
<xml_diff>
--- a/Finished/Chewy/Chewy 856 ASN PO RS41334490 11.08.2024.xlsx
+++ b/Finished/Chewy/Chewy 856 ASN PO RS41334490 11.08.2024.xlsx
@@ -1272,7 +1272,11 @@
           <t>1358182</t>
         </is>
       </c>
-      <c r="H21" s="33" t="n"/>
+      <c r="H21" s="33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I21" s="33" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1316,7 +1320,11 @@
           <t>1358182</t>
         </is>
       </c>
-      <c r="H22" s="33" t="n"/>
+      <c r="H22" s="33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I22" s="33" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1360,7 +1368,11 @@
           <t>1358182</t>
         </is>
       </c>
-      <c r="H23" s="33" t="n"/>
+      <c r="H23" s="33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I23" s="33" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1403,6 +1415,11 @@
           <t>1358182</t>
         </is>
       </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1443,6 +1460,11 @@
           <t>1358182</t>
         </is>
       </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I25" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1483,6 +1505,11 @@
           <t>1358174</t>
         </is>
       </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I26" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1523,6 +1550,11 @@
           <t>1358238</t>
         </is>
       </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I27" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1563,6 +1595,11 @@
           <t>1358318</t>
         </is>
       </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I28" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1603,6 +1640,11 @@
           <t>1358454</t>
         </is>
       </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I29" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1643,6 +1685,11 @@
           <t>1358462</t>
         </is>
       </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I30" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1683,6 +1730,11 @@
           <t>1358494</t>
         </is>
       </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="I31" t="inlineStr">
         <is>
           <t>CA</t>
@@ -1721,6 +1773,11 @@
       <c r="G32" t="inlineStr">
         <is>
           <t>1358518</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">

</xml_diff>